<commit_message>
Tweak formatting of charts and add Excel charts
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://morpc1-my.sharepoint.com/personal/aporr_morpc_org/Documents/renewenergy-der-facilities/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_226563EAB0730FA183037501310F05FD797BF70E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D1BAFBB-33B0-4D1B-A195-C7BB30FB7E4A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1033,8 +1027,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1110,21 +1104,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1162,7 +1148,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1196,7 +1182,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1231,10 +1216,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1407,20 +1391,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A157" sqref="A2:XFD157"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="126.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -1499,7 +1477,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1534,7 +1512,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -1569,7 +1547,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1604,7 +1582,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -1639,7 +1617,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -1674,7 +1652,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +1687,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -1744,7 +1722,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -1779,7 +1757,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1814,7 +1792,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -1849,7 +1827,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14">
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -1884,7 +1862,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -1919,7 +1897,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1954,7 +1932,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -1989,7 +1967,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -2024,7 +2002,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -2059,7 +2037,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -2094,7 +2072,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14">
       <c r="B20" t="s">
         <v>14</v>
       </c>
@@ -2129,7 +2107,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14">
       <c r="B21" t="s">
         <v>14</v>
       </c>
@@ -2164,7 +2142,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14">
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -2199,7 +2177,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14">
       <c r="B23" t="s">
         <v>14</v>
       </c>
@@ -2234,7 +2212,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -2269,7 +2247,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14">
       <c r="B25" t="s">
         <v>14</v>
       </c>
@@ -2304,7 +2282,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14">
       <c r="B26" t="s">
         <v>14</v>
       </c>
@@ -2339,7 +2317,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14">
       <c r="B27" t="s">
         <v>14</v>
       </c>
@@ -2374,7 +2352,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -2409,7 +2387,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14">
       <c r="B29" t="s">
         <v>14</v>
       </c>
@@ -2444,7 +2422,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14">
       <c r="B30" t="s">
         <v>14</v>
       </c>
@@ -2479,7 +2457,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14">
       <c r="B31" t="s">
         <v>14</v>
       </c>
@@ -2514,7 +2492,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14">
       <c r="B32" t="s">
         <v>14</v>
       </c>
@@ -2549,7 +2527,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14">
       <c r="B33" t="s">
         <v>14</v>
       </c>
@@ -2584,7 +2562,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14">
       <c r="B34" t="s">
         <v>14</v>
       </c>
@@ -2619,7 +2597,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14">
       <c r="B35" t="s">
         <v>14</v>
       </c>
@@ -2654,7 +2632,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14">
       <c r="B36" t="s">
         <v>14</v>
       </c>
@@ -2689,7 +2667,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14">
       <c r="B37" t="s">
         <v>14</v>
       </c>
@@ -2724,7 +2702,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14">
       <c r="B38" t="s">
         <v>14</v>
       </c>
@@ -2759,7 +2737,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14">
       <c r="B39" t="s">
         <v>14</v>
       </c>
@@ -2794,7 +2772,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14">
       <c r="B40" t="s">
         <v>14</v>
       </c>
@@ -2829,7 +2807,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14">
       <c r="B41" t="s">
         <v>14</v>
       </c>
@@ -2864,7 +2842,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14">
       <c r="B42" t="s">
         <v>14</v>
       </c>
@@ -2899,7 +2877,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:14">
       <c r="B43" t="s">
         <v>14</v>
       </c>
@@ -2934,7 +2912,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:14">
       <c r="B44" t="s">
         <v>14</v>
       </c>
@@ -2969,7 +2947,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:14">
       <c r="B45" t="s">
         <v>14</v>
       </c>
@@ -3004,7 +2982,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:14">
       <c r="B46" t="s">
         <v>14</v>
       </c>
@@ -3039,7 +3017,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:14">
       <c r="B47" t="s">
         <v>14</v>
       </c>
@@ -3074,7 +3052,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:14">
       <c r="B48" t="s">
         <v>14</v>
       </c>
@@ -3109,7 +3087,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:14">
       <c r="B49" t="s">
         <v>14</v>
       </c>
@@ -3144,7 +3122,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:14">
       <c r="B50" t="s">
         <v>14</v>
       </c>
@@ -3179,7 +3157,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:14">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -3214,7 +3192,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:14">
       <c r="B52" t="s">
         <v>14</v>
       </c>
@@ -3249,7 +3227,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:14">
       <c r="B53" t="s">
         <v>14</v>
       </c>
@@ -3284,7 +3262,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:14">
       <c r="B54" t="s">
         <v>14</v>
       </c>
@@ -3319,7 +3297,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:14">
       <c r="B55" t="s">
         <v>14</v>
       </c>
@@ -3354,7 +3332,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:14">
       <c r="B56" t="s">
         <v>14</v>
       </c>
@@ -3389,7 +3367,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:14">
       <c r="B57" t="s">
         <v>14</v>
       </c>
@@ -3424,7 +3402,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:14">
       <c r="B58" t="s">
         <v>14</v>
       </c>
@@ -3459,7 +3437,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:14">
       <c r="B59" t="s">
         <v>14</v>
       </c>
@@ -3494,7 +3472,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:14">
       <c r="B60" t="s">
         <v>14</v>
       </c>
@@ -3529,7 +3507,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:14">
       <c r="B61" t="s">
         <v>14</v>
       </c>
@@ -3564,7 +3542,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:14">
       <c r="B62" t="s">
         <v>14</v>
       </c>
@@ -3599,7 +3577,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:14">
       <c r="B63" t="s">
         <v>14</v>
       </c>
@@ -3634,7 +3612,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:14">
       <c r="B64" t="s">
         <v>14</v>
       </c>
@@ -3669,7 +3647,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:14">
       <c r="B65" t="s">
         <v>14</v>
       </c>
@@ -3704,7 +3682,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:14">
       <c r="B66" t="s">
         <v>14</v>
       </c>
@@ -3739,7 +3717,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:14">
       <c r="B67" t="s">
         <v>14</v>
       </c>
@@ -3774,7 +3752,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:14">
       <c r="B68" t="s">
         <v>14</v>
       </c>
@@ -3809,7 +3787,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:14">
       <c r="B69" t="s">
         <v>14</v>
       </c>
@@ -3844,7 +3822,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:14">
       <c r="B70" t="s">
         <v>14</v>
       </c>
@@ -3879,7 +3857,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:14">
       <c r="B71" t="s">
         <v>14</v>
       </c>
@@ -3914,7 +3892,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:14">
       <c r="B72" t="s">
         <v>14</v>
       </c>
@@ -3949,7 +3927,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:14">
       <c r="B73" t="s">
         <v>14</v>
       </c>
@@ -3984,7 +3962,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:14">
       <c r="B74" t="s">
         <v>14</v>
       </c>
@@ -4019,7 +3997,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:14">
       <c r="B75" t="s">
         <v>14</v>
       </c>
@@ -4054,7 +4032,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:14">
       <c r="B76" t="s">
         <v>14</v>
       </c>
@@ -4089,7 +4067,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:14">
       <c r="B77" t="s">
         <v>14</v>
       </c>
@@ -4124,7 +4102,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:14">
       <c r="B78" t="s">
         <v>14</v>
       </c>
@@ -4159,7 +4137,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:14">
       <c r="B79" t="s">
         <v>14</v>
       </c>
@@ -4194,7 +4172,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:14">
       <c r="B80" t="s">
         <v>15</v>
       </c>
@@ -4229,7 +4207,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:14">
       <c r="B81" t="s">
         <v>15</v>
       </c>
@@ -4264,7 +4242,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:14">
       <c r="B82" t="s">
         <v>15</v>
       </c>
@@ -4299,7 +4277,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:14">
       <c r="B83" t="s">
         <v>15</v>
       </c>
@@ -4334,7 +4312,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:14">
       <c r="B84" t="s">
         <v>15</v>
       </c>
@@ -4369,7 +4347,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:14">
       <c r="B85" t="s">
         <v>15</v>
       </c>
@@ -4404,7 +4382,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:14">
       <c r="B86" t="s">
         <v>15</v>
       </c>
@@ -4439,7 +4417,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:14">
       <c r="B87" t="s">
         <v>15</v>
       </c>
@@ -4474,7 +4452,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:14">
       <c r="B88" t="s">
         <v>15</v>
       </c>
@@ -4509,7 +4487,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:14">
       <c r="B89" t="s">
         <v>15</v>
       </c>
@@ -4544,7 +4522,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:14">
       <c r="B90" t="s">
         <v>15</v>
       </c>
@@ -4579,7 +4557,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:14">
       <c r="B91" t="s">
         <v>15</v>
       </c>
@@ -4614,7 +4592,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:14">
       <c r="B92" t="s">
         <v>15</v>
       </c>
@@ -4649,7 +4627,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:14">
       <c r="B93" t="s">
         <v>15</v>
       </c>
@@ -4684,7 +4662,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:14">
       <c r="B94" t="s">
         <v>15</v>
       </c>
@@ -4719,7 +4697,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:14">
       <c r="B95" t="s">
         <v>15</v>
       </c>
@@ -4754,7 +4732,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:14">
       <c r="B96" t="s">
         <v>15</v>
       </c>
@@ -4789,7 +4767,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:14">
       <c r="B97" t="s">
         <v>15</v>
       </c>
@@ -4824,7 +4802,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:14">
       <c r="B98" t="s">
         <v>15</v>
       </c>
@@ -4859,7 +4837,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:14">
       <c r="B99" t="s">
         <v>15</v>
       </c>
@@ -4894,7 +4872,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:14">
       <c r="B100" t="s">
         <v>15</v>
       </c>
@@ -4929,7 +4907,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:14">
       <c r="B101" t="s">
         <v>15</v>
       </c>
@@ -4964,7 +4942,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:14">
       <c r="B102" t="s">
         <v>15</v>
       </c>
@@ -4999,7 +4977,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:14">
       <c r="B103" t="s">
         <v>15</v>
       </c>
@@ -5034,7 +5012,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:14">
       <c r="B104" t="s">
         <v>15</v>
       </c>
@@ -5069,7 +5047,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:14">
       <c r="B105" t="s">
         <v>15</v>
       </c>
@@ -5104,7 +5082,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:14">
       <c r="B106" t="s">
         <v>15</v>
       </c>
@@ -5139,7 +5117,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:14">
       <c r="B107" t="s">
         <v>15</v>
       </c>
@@ -5174,7 +5152,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:14">
       <c r="B108" t="s">
         <v>15</v>
       </c>
@@ -5209,7 +5187,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:14">
       <c r="B109" t="s">
         <v>15</v>
       </c>
@@ -5244,7 +5222,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:14">
       <c r="B110" t="s">
         <v>15</v>
       </c>
@@ -5279,7 +5257,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:14">
       <c r="B111" t="s">
         <v>15</v>
       </c>
@@ -5314,7 +5292,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:14">
       <c r="B112" t="s">
         <v>15</v>
       </c>
@@ -5349,7 +5327,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:14">
       <c r="B113" t="s">
         <v>15</v>
       </c>
@@ -5384,7 +5362,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="114" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:14">
       <c r="B114" t="s">
         <v>15</v>
       </c>
@@ -5419,7 +5397,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="115" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:14">
       <c r="B115" t="s">
         <v>15</v>
       </c>
@@ -5454,7 +5432,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="116" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:14">
       <c r="B116" t="s">
         <v>15</v>
       </c>
@@ -5489,7 +5467,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="117" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:14">
       <c r="B117" t="s">
         <v>15</v>
       </c>
@@ -5524,7 +5502,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="118" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:14">
       <c r="B118" t="s">
         <v>15</v>
       </c>
@@ -5559,7 +5537,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="119" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:14">
       <c r="B119" t="s">
         <v>15</v>
       </c>
@@ -5594,7 +5572,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="120" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:14">
       <c r="B120" t="s">
         <v>15</v>
       </c>
@@ -5629,7 +5607,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:14">
       <c r="B121" t="s">
         <v>15</v>
       </c>
@@ -5664,7 +5642,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="122" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:14">
       <c r="B122" t="s">
         <v>15</v>
       </c>
@@ -5699,7 +5677,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="123" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:14">
       <c r="B123" t="s">
         <v>15</v>
       </c>
@@ -5734,7 +5712,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="124" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:14">
       <c r="B124" t="s">
         <v>15</v>
       </c>
@@ -5769,7 +5747,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="125" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:14">
       <c r="B125" t="s">
         <v>15</v>
       </c>
@@ -5804,7 +5782,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="126" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:14">
       <c r="B126" t="s">
         <v>15</v>
       </c>
@@ -5839,7 +5817,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="127" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:14">
       <c r="B127" t="s">
         <v>15</v>
       </c>
@@ -5874,7 +5852,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="128" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:14">
       <c r="B128" t="s">
         <v>15</v>
       </c>
@@ -5909,7 +5887,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="129" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:14">
       <c r="B129" t="s">
         <v>15</v>
       </c>
@@ -5944,7 +5922,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="130" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:14">
       <c r="B130" t="s">
         <v>15</v>
       </c>
@@ -5979,7 +5957,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="131" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:14">
       <c r="B131" t="s">
         <v>15</v>
       </c>
@@ -6014,7 +5992,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="132" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:14">
       <c r="B132" t="s">
         <v>15</v>
       </c>
@@ -6049,7 +6027,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="133" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:14">
       <c r="B133" t="s">
         <v>15</v>
       </c>
@@ -6084,7 +6062,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="134" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:14">
       <c r="B134" t="s">
         <v>15</v>
       </c>
@@ -6119,7 +6097,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="135" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:14">
       <c r="B135" t="s">
         <v>15</v>
       </c>
@@ -6154,7 +6132,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="136" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:14">
       <c r="B136" t="s">
         <v>15</v>
       </c>
@@ -6189,7 +6167,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="137" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:14">
       <c r="B137" t="s">
         <v>15</v>
       </c>
@@ -6224,7 +6202,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="138" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:14">
       <c r="B138" t="s">
         <v>15</v>
       </c>
@@ -6259,7 +6237,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="139" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:14">
       <c r="B139" t="s">
         <v>15</v>
       </c>
@@ -6294,7 +6272,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="140" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:14">
       <c r="B140" t="s">
         <v>15</v>
       </c>
@@ -6329,7 +6307,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="141" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:14">
       <c r="B141" t="s">
         <v>15</v>
       </c>
@@ -6364,7 +6342,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="142" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:14">
       <c r="B142" t="s">
         <v>15</v>
       </c>
@@ -6399,7 +6377,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="143" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:14">
       <c r="B143" t="s">
         <v>15</v>
       </c>
@@ -6434,7 +6412,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="144" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:14">
       <c r="B144" t="s">
         <v>15</v>
       </c>
@@ -6469,7 +6447,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="145" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:14">
       <c r="B145" t="s">
         <v>15</v>
       </c>
@@ -6504,7 +6482,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="146" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:14">
       <c r="B146" t="s">
         <v>15</v>
       </c>
@@ -6539,7 +6517,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="147" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:14">
       <c r="B147" t="s">
         <v>15</v>
       </c>
@@ -6574,7 +6552,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="148" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:14">
       <c r="B148" t="s">
         <v>15</v>
       </c>
@@ -6609,7 +6587,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="149" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:14">
       <c r="B149" t="s">
         <v>15</v>
       </c>
@@ -6644,7 +6622,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="150" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:14">
       <c r="B150" t="s">
         <v>15</v>
       </c>
@@ -6679,7 +6657,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="151" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:14">
       <c r="B151" t="s">
         <v>15</v>
       </c>
@@ -6714,7 +6692,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="152" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:14">
       <c r="B152" t="s">
         <v>15</v>
       </c>
@@ -6749,7 +6727,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="153" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:14">
       <c r="B153" t="s">
         <v>15</v>
       </c>
@@ -6784,7 +6762,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="154" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:14">
       <c r="B154" t="s">
         <v>15</v>
       </c>
@@ -6819,7 +6797,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="155" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:14">
       <c r="B155" t="s">
         <v>15</v>
       </c>
@@ -6854,7 +6832,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="156" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:14">
       <c r="B156" t="s">
         <v>15</v>
       </c>
@@ -6889,7 +6867,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="157" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:14">
       <c r="B157" t="s">
         <v>15</v>
       </c>
@@ -6926,474 +6904,474 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="M2" r:id="rId2" location="geoid=0500000US39041" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="N2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="M3" r:id="rId5" location="geoid=0500000US39045" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="N3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="M4" r:id="rId8" location="geoid=0500000US39047" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="N4" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H5" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="M5" r:id="rId11" location="geoid=0500000US39049" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="N5" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="H6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="M6" r:id="rId14" location="geoid=0500000US39073" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="N6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="M7" r:id="rId17" location="geoid=0500000US39083" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="N7" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="H8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="M8" r:id="rId20" location="geoid=0500000US39089" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="N8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="H9" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="M9" r:id="rId23" location="geoid=0500000US39091" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="N9" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="H10" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="M10" r:id="rId26" location="geoid=0500000US39097" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="N10" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="H11" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="M11" r:id="rId29" location="geoid=0500000US39101" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="N11" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H12" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="M12" r:id="rId32" location="geoid=0500000US39117" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="N12" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="H13" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="M13" r:id="rId35" location="geoid=0500000US39127" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="N13" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H14" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="M14" r:id="rId38" location="geoid=0500000US39129" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="N14" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="H15" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="M15" r:id="rId41" location="geoid=0500000US39141" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="N15" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="H16" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="M16" r:id="rId44" location="geoid=0500000US39159" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="N16" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="H17" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="M17" r:id="rId47" location="geoid=0700000US390458020699999" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="N17" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="H18" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="M18" r:id="rId50" location="geoid=0700000US390490692299999" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="N18" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="H19" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="M19" r:id="rId53" location="geoid=0700000US390490944299999" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="N19" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="H20" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="M20" r:id="rId56" location="geoid=0700000US390491611299999" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="N20" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="H21" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="M21" r:id="rId59" location="geoid=0700000US390492828099999" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="N21" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="H22" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="M22" r:id="rId62" location="geoid=0700000US390493777299999" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="N22" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="H23" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="M23" r:id="rId65" location="geoid=0700000US390493861299999" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="N23" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="H24" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="M24" r:id="rId68" location="geoid=0700000US390494641099999" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="N24" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="H25" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="M25" r:id="rId71" location="geoid=0700000US390495006499999" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="N25" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="H26" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="M26" r:id="rId74" location="geoid=0700000US390496184099999" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="N26" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="H27" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="M27" r:id="rId77" location="geoid=0700000US390496297499999" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="N27" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="H28" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="M28" r:id="rId80" location="geoid=0700000US390496457099999" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="N28" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="H29" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="M29" r:id="rId83" location="geoid=0700000US390497771499999" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="N29" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="H30" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="M30" r:id="rId86" location="geoid=0700000US390498124299999" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="N30" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="H31" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="M31" r:id="rId89" location="geoid=0700000US390892569099999" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="N31" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="H32" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="M32" r:id="rId92" location="geoid=0700000US390893141699999" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="N32" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="H33" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="M33" r:id="rId95" location="geoid=0700000US391593904699999" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="N33" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="H34" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="M34" r:id="rId98" location="geoid=1600000US3905130" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="N34" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="H35" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="M35" r:id="rId101" location="geoid=1600000US3906278" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="N35" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="H36" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="M36" r:id="rId104" location="geoid=1600000US3909890" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="N36" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="H37" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="M37" r:id="rId107" location="geoid=1600000US3914184" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="N37" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="H38" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="M38" r:id="rId110" location="geoid=1600000US3915070" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="N38" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="H39" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="M39" r:id="rId113" location="geoid=1600000US3918000" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="N39" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="H40" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="M40" r:id="rId116" location="geoid=1600000US3921434" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="N40" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="H41" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="M41" r:id="rId119" location="geoid=1600000US3922694" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="N41" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="H42" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="M42" r:id="rId122" location="geoid=1600000US3929106" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="N42" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="H43" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="M43" r:id="rId125" location="geoid=1600000US3929148" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="N43" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="H44" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="M44" r:id="rId128" location="geoid=1600000US3929246" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="N44" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="H45" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="M45" r:id="rId131" location="geoid=1600000US3931304" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="N45" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="H46" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="M46" r:id="rId134" location="geoid=1600000US3931402" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="N46" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="H47" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="M47" r:id="rId137" location="geoid=1600000US3932592" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="N47" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="H48" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="M48" r:id="rId140" location="geoid=1600000US3932606" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="N48" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="H49" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="M49" r:id="rId143" location="geoid=1600000US3934748" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="N49" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="H50" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="M50" r:id="rId146" location="geoid=1600000US3934790" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="N50" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="H51" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="M51" r:id="rId149" location="geoid=1600000US3935476" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="N51" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="H52" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="M52" r:id="rId152" location="geoid=1600000US3939340" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="N52" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="H53" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="M53" r:id="rId155" location="geoid=1600000US3941720" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="N53" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="H54" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="M54" r:id="rId158" location="geoid=1600000US3944674" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="N54" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="H55" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="M55" r:id="rId161" location="geoid=1600000US3947474" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="N55" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="H56" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="M56" r:id="rId164" location="geoid=1600000US3947754" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="N56" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="H57" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="M57" r:id="rId167" location="geoid=1600000US3948160" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="N57" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="H58" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="M58" r:id="rId170" location="geoid=1600000US3950862" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="N58" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="H59" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="M59" r:id="rId173" location="geoid=1600000US3953046" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="N59" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="H60" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="M60" r:id="rId176" location="geoid=1600000US3953102" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="N60" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="H61" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="M61" r:id="rId179" location="geoid=1600000US3953970" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="N61" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="H62" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="M62" r:id="rId182" location="geoid=1600000US3954040" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="N62" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="H63" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="M63" r:id="rId185" location="geoid=1600000US3954866" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="N63" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="H64" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="M64" r:id="rId188" location="geoid=1600000US3957862" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="N64" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="H65" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="M65" r:id="rId191" location="geoid=1600000US3961112" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="N65" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="H66" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="M66" r:id="rId194" location="geoid=1600000US3962498" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="N66" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="H67" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="M67" r:id="rId197" location="geoid=1600000US3963030" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="N67" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="H68" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="M68" r:id="rId200" location="geoid=1600000US3964486" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="N68" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="H69" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="M69" r:id="rId203" location="geoid=1600000US3966390" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="N69" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="H70" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="M70" r:id="rId206" location="geoid=1600000US3967440" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="N70" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="H71" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="M71" r:id="rId209" location="geoid=1600000US3971976" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="N71" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="H72" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="M72" r:id="rId212" location="geoid=1600000US3972977" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="N72" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="H73" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="M73" r:id="rId215" location="geoid=1600000US3975602" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="N73" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="H74" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="M74" r:id="rId218" location="geoid=1600000US3979002" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="N74" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="H75" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="M75" r:id="rId221" location="geoid=1600000US3979100" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="N75" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="H76" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="M76" r:id="rId224" location="geoid=1600000US3983580" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="N76" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="H77" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="M77" r:id="rId227" location="geoid=1600000US3984742" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="N77" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="H78" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="M78" r:id="rId230" location="geoid=1600000US3986604" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="N78" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="H79" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="M79" r:id="rId233" location="geoid=M010000US001" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="N79" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="H80" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="M80" r:id="rId236" location="geoid=0500000US39041" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="N80" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="H81" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="M81" r:id="rId239" location="geoid=0500000US39045" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="N81" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="H82" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="M82" r:id="rId242" location="geoid=0500000US39047" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="N82" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="H83" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="M83" r:id="rId245" location="geoid=0500000US39049" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="N83" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="H84" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="M84" r:id="rId248" location="geoid=0500000US39073" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="N84" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="H85" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="M85" r:id="rId251" location="geoid=0500000US39083" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="N85" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="H86" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="M86" r:id="rId254" location="geoid=0500000US39089" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="N86" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="H87" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="M87" r:id="rId257" location="geoid=0500000US39091" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="N87" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="H88" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="M88" r:id="rId260" location="geoid=0500000US39097" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="N88" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="H89" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="M89" r:id="rId263" location="geoid=0500000US39101" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="N89" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="H90" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="M90" r:id="rId266" location="geoid=0500000US39117" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="N90" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="H91" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="M91" r:id="rId269" location="geoid=0500000US39127" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="N91" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="H92" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="M92" r:id="rId272" location="geoid=0500000US39129" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="N92" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="H93" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="M93" r:id="rId275" location="geoid=0500000US39141" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="N93" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="H94" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="M94" r:id="rId278" location="geoid=0500000US39159" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="N94" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="H95" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="M95" r:id="rId281" location="geoid=0700000US390458020699999" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="N95" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="H96" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="M96" r:id="rId284" location="geoid=0700000US390490692299999" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="N96" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="H97" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="M97" r:id="rId287" location="geoid=0700000US390490944299999" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="N97" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="H98" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="M98" r:id="rId290" location="geoid=0700000US390491611299999" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="N98" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="H99" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="M99" r:id="rId293" location="geoid=0700000US390492828099999" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="N99" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="H100" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="M100" r:id="rId296" location="geoid=0700000US390493777299999" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="N100" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="H101" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="M101" r:id="rId299" location="geoid=0700000US390493861299999" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="N101" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="H102" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="M102" r:id="rId302" location="geoid=0700000US390494641099999" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="N102" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="H103" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="M103" r:id="rId305" location="geoid=0700000US390495006499999" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="N103" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="H104" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="M104" r:id="rId308" location="geoid=0700000US390496184099999" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="N104" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="H105" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="M105" r:id="rId311" location="geoid=0700000US390496297499999" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="N105" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="H106" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="M106" r:id="rId314" location="geoid=0700000US390496457099999" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="N106" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="H107" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="M107" r:id="rId317" location="geoid=0700000US390497771499999" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="N107" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="H108" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="M108" r:id="rId320" location="geoid=0700000US390498124299999" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="N108" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="H109" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="M109" r:id="rId323" location="geoid=0700000US390892569099999" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="N109" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="H110" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="M110" r:id="rId326" location="geoid=0700000US390893141699999" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="N110" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="H111" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="M111" r:id="rId329" location="geoid=0700000US391593904699999" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="N111" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="H112" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="M112" r:id="rId332" location="geoid=1600000US3905130" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="N112" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="H113" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="M113" r:id="rId335" location="geoid=1600000US3906278" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="N113" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="H114" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="M114" r:id="rId338" location="geoid=1600000US3909890" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="N114" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="H115" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="M115" r:id="rId341" location="geoid=1600000US3914184" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="N115" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="H116" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="M116" r:id="rId344" location="geoid=1600000US3915070" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="N116" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="H117" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="M117" r:id="rId347" location="geoid=1600000US3918000" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="N117" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="H118" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="M118" r:id="rId350" location="geoid=1600000US3921434" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="N118" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="H119" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="M119" r:id="rId353" location="geoid=1600000US3922694" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="N119" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="H120" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="M120" r:id="rId356" location="geoid=1600000US3929106" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="N120" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="H121" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
-    <hyperlink ref="M121" r:id="rId359" location="geoid=1600000US3929148" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="N121" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="H122" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="M122" r:id="rId362" location="geoid=1600000US3929246" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
-    <hyperlink ref="N122" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
-    <hyperlink ref="H123" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
-    <hyperlink ref="M123" r:id="rId365" location="geoid=1600000US3931304" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
-    <hyperlink ref="N123" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
-    <hyperlink ref="H124" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
-    <hyperlink ref="M124" r:id="rId368" location="geoid=1600000US3931402" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
-    <hyperlink ref="N124" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
-    <hyperlink ref="H125" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
-    <hyperlink ref="M125" r:id="rId371" location="geoid=1600000US3932592" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
-    <hyperlink ref="N125" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
-    <hyperlink ref="H126" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
-    <hyperlink ref="M126" r:id="rId374" location="geoid=1600000US3932606" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
-    <hyperlink ref="N126" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
-    <hyperlink ref="H127" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
-    <hyperlink ref="M127" r:id="rId377" location="geoid=1600000US3934748" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
-    <hyperlink ref="N127" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
-    <hyperlink ref="H128" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
-    <hyperlink ref="M128" r:id="rId380" location="geoid=1600000US3934790" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
-    <hyperlink ref="N128" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
-    <hyperlink ref="H129" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
-    <hyperlink ref="M129" r:id="rId383" location="geoid=1600000US3935476" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
-    <hyperlink ref="N129" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
-    <hyperlink ref="H130" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
-    <hyperlink ref="M130" r:id="rId386" location="geoid=1600000US3939340" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
-    <hyperlink ref="N130" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
-    <hyperlink ref="H131" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
-    <hyperlink ref="M131" r:id="rId389" location="geoid=1600000US3941720" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
-    <hyperlink ref="N131" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
-    <hyperlink ref="H132" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
-    <hyperlink ref="M132" r:id="rId392" location="geoid=1600000US3944674" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
-    <hyperlink ref="N132" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
-    <hyperlink ref="H133" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
-    <hyperlink ref="M133" r:id="rId395" location="geoid=1600000US3947474" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
-    <hyperlink ref="N133" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
-    <hyperlink ref="H134" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="M134" r:id="rId398" location="geoid=1600000US3947754" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
-    <hyperlink ref="N134" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
-    <hyperlink ref="H135" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
-    <hyperlink ref="M135" r:id="rId401" location="geoid=1600000US3948160" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
-    <hyperlink ref="N135" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
-    <hyperlink ref="H136" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
-    <hyperlink ref="M136" r:id="rId404" location="geoid=1600000US3950862" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
-    <hyperlink ref="N136" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
-    <hyperlink ref="H137" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
-    <hyperlink ref="M137" r:id="rId407" location="geoid=1600000US3953046" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
-    <hyperlink ref="N137" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
-    <hyperlink ref="H138" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
-    <hyperlink ref="M138" r:id="rId410" location="geoid=1600000US3953102" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
-    <hyperlink ref="N138" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
-    <hyperlink ref="H139" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
-    <hyperlink ref="M139" r:id="rId413" location="geoid=1600000US3953970" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
-    <hyperlink ref="N139" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
-    <hyperlink ref="H140" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
-    <hyperlink ref="M140" r:id="rId416" location="geoid=1600000US3954040" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
-    <hyperlink ref="N140" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
-    <hyperlink ref="H141" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
-    <hyperlink ref="M141" r:id="rId419" location="geoid=1600000US3954866" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
-    <hyperlink ref="N141" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
-    <hyperlink ref="H142" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
-    <hyperlink ref="M142" r:id="rId422" location="geoid=1600000US3957862" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
-    <hyperlink ref="N142" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
-    <hyperlink ref="H143" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
-    <hyperlink ref="M143" r:id="rId425" location="geoid=1600000US3961112" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
-    <hyperlink ref="N143" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
-    <hyperlink ref="H144" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
-    <hyperlink ref="M144" r:id="rId428" location="geoid=1600000US3962498" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
-    <hyperlink ref="N144" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
-    <hyperlink ref="H145" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
-    <hyperlink ref="M145" r:id="rId431" location="geoid=1600000US3963030" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
-    <hyperlink ref="N145" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
-    <hyperlink ref="H146" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
-    <hyperlink ref="M146" r:id="rId434" location="geoid=1600000US3964486" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
-    <hyperlink ref="N146" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
-    <hyperlink ref="H147" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
-    <hyperlink ref="M147" r:id="rId437" location="geoid=1600000US3966390" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
-    <hyperlink ref="N147" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
-    <hyperlink ref="H148" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
-    <hyperlink ref="M148" r:id="rId440" location="geoid=1600000US3967440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
-    <hyperlink ref="N148" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
-    <hyperlink ref="H149" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
-    <hyperlink ref="M149" r:id="rId443" location="geoid=1600000US3971976" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
-    <hyperlink ref="N149" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
-    <hyperlink ref="H150" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
-    <hyperlink ref="M150" r:id="rId446" location="geoid=1600000US3972977" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
-    <hyperlink ref="N150" r:id="rId447" xr:uid="{00000000-0004-0000-0000-0000BE010000}"/>
-    <hyperlink ref="H151" r:id="rId448" xr:uid="{00000000-0004-0000-0000-0000BF010000}"/>
-    <hyperlink ref="M151" r:id="rId449" location="geoid=1600000US3975602" xr:uid="{00000000-0004-0000-0000-0000C0010000}"/>
-    <hyperlink ref="N151" r:id="rId450" xr:uid="{00000000-0004-0000-0000-0000C1010000}"/>
-    <hyperlink ref="H152" r:id="rId451" xr:uid="{00000000-0004-0000-0000-0000C2010000}"/>
-    <hyperlink ref="M152" r:id="rId452" location="geoid=1600000US3979002" xr:uid="{00000000-0004-0000-0000-0000C3010000}"/>
-    <hyperlink ref="N152" r:id="rId453" xr:uid="{00000000-0004-0000-0000-0000C4010000}"/>
-    <hyperlink ref="H153" r:id="rId454" xr:uid="{00000000-0004-0000-0000-0000C5010000}"/>
-    <hyperlink ref="M153" r:id="rId455" location="geoid=1600000US3979100" xr:uid="{00000000-0004-0000-0000-0000C6010000}"/>
-    <hyperlink ref="N153" r:id="rId456" xr:uid="{00000000-0004-0000-0000-0000C7010000}"/>
-    <hyperlink ref="H154" r:id="rId457" xr:uid="{00000000-0004-0000-0000-0000C8010000}"/>
-    <hyperlink ref="M154" r:id="rId458" location="geoid=1600000US3983580" xr:uid="{00000000-0004-0000-0000-0000C9010000}"/>
-    <hyperlink ref="N154" r:id="rId459" xr:uid="{00000000-0004-0000-0000-0000CA010000}"/>
-    <hyperlink ref="H155" r:id="rId460" xr:uid="{00000000-0004-0000-0000-0000CB010000}"/>
-    <hyperlink ref="M155" r:id="rId461" location="geoid=1600000US3984742" xr:uid="{00000000-0004-0000-0000-0000CC010000}"/>
-    <hyperlink ref="N155" r:id="rId462" xr:uid="{00000000-0004-0000-0000-0000CD010000}"/>
-    <hyperlink ref="H156" r:id="rId463" xr:uid="{00000000-0004-0000-0000-0000CE010000}"/>
-    <hyperlink ref="M156" r:id="rId464" location="geoid=1600000US3986604" xr:uid="{00000000-0004-0000-0000-0000CF010000}"/>
-    <hyperlink ref="N156" r:id="rId465" xr:uid="{00000000-0004-0000-0000-0000D0010000}"/>
-    <hyperlink ref="H157" r:id="rId466" xr:uid="{00000000-0004-0000-0000-0000D1010000}"/>
-    <hyperlink ref="M157" r:id="rId467" location="geoid=M010000US001" xr:uid="{00000000-0004-0000-0000-0000D2010000}"/>
-    <hyperlink ref="N157" r:id="rId468" xr:uid="{00000000-0004-0000-0000-0000D3010000}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId2" location="geoid=0500000US39041"/>
+    <hyperlink ref="N2" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="M3" r:id="rId5" location="geoid=0500000US39045"/>
+    <hyperlink ref="N3" r:id="rId6"/>
+    <hyperlink ref="H4" r:id="rId7"/>
+    <hyperlink ref="M4" r:id="rId8" location="geoid=0500000US39047"/>
+    <hyperlink ref="N4" r:id="rId9"/>
+    <hyperlink ref="H5" r:id="rId10"/>
+    <hyperlink ref="M5" r:id="rId11" location="geoid=0500000US39049"/>
+    <hyperlink ref="N5" r:id="rId12"/>
+    <hyperlink ref="H6" r:id="rId13"/>
+    <hyperlink ref="M6" r:id="rId14" location="geoid=0500000US39073"/>
+    <hyperlink ref="N6" r:id="rId15"/>
+    <hyperlink ref="H7" r:id="rId16"/>
+    <hyperlink ref="M7" r:id="rId17" location="geoid=0500000US39083"/>
+    <hyperlink ref="N7" r:id="rId18"/>
+    <hyperlink ref="H8" r:id="rId19"/>
+    <hyperlink ref="M8" r:id="rId20" location="geoid=0500000US39089"/>
+    <hyperlink ref="N8" r:id="rId21"/>
+    <hyperlink ref="H9" r:id="rId22"/>
+    <hyperlink ref="M9" r:id="rId23" location="geoid=0500000US39091"/>
+    <hyperlink ref="N9" r:id="rId24"/>
+    <hyperlink ref="H10" r:id="rId25"/>
+    <hyperlink ref="M10" r:id="rId26" location="geoid=0500000US39097"/>
+    <hyperlink ref="N10" r:id="rId27"/>
+    <hyperlink ref="H11" r:id="rId28"/>
+    <hyperlink ref="M11" r:id="rId29" location="geoid=0500000US39101"/>
+    <hyperlink ref="N11" r:id="rId30"/>
+    <hyperlink ref="H12" r:id="rId31"/>
+    <hyperlink ref="M12" r:id="rId32" location="geoid=0500000US39117"/>
+    <hyperlink ref="N12" r:id="rId33"/>
+    <hyperlink ref="H13" r:id="rId34"/>
+    <hyperlink ref="M13" r:id="rId35" location="geoid=0500000US39127"/>
+    <hyperlink ref="N13" r:id="rId36"/>
+    <hyperlink ref="H14" r:id="rId37"/>
+    <hyperlink ref="M14" r:id="rId38" location="geoid=0500000US39129"/>
+    <hyperlink ref="N14" r:id="rId39"/>
+    <hyperlink ref="H15" r:id="rId40"/>
+    <hyperlink ref="M15" r:id="rId41" location="geoid=0500000US39141"/>
+    <hyperlink ref="N15" r:id="rId42"/>
+    <hyperlink ref="H16" r:id="rId43"/>
+    <hyperlink ref="M16" r:id="rId44" location="geoid=0500000US39159"/>
+    <hyperlink ref="N16" r:id="rId45"/>
+    <hyperlink ref="H17" r:id="rId46"/>
+    <hyperlink ref="M17" r:id="rId47" location="geoid=0700000US390458020699999"/>
+    <hyperlink ref="N17" r:id="rId48"/>
+    <hyperlink ref="H18" r:id="rId49"/>
+    <hyperlink ref="M18" r:id="rId50" location="geoid=0700000US390490692299999"/>
+    <hyperlink ref="N18" r:id="rId51"/>
+    <hyperlink ref="H19" r:id="rId52"/>
+    <hyperlink ref="M19" r:id="rId53" location="geoid=0700000US390490944299999"/>
+    <hyperlink ref="N19" r:id="rId54"/>
+    <hyperlink ref="H20" r:id="rId55"/>
+    <hyperlink ref="M20" r:id="rId56" location="geoid=0700000US390491611299999"/>
+    <hyperlink ref="N20" r:id="rId57"/>
+    <hyperlink ref="H21" r:id="rId58"/>
+    <hyperlink ref="M21" r:id="rId59" location="geoid=0700000US390492828099999"/>
+    <hyperlink ref="N21" r:id="rId60"/>
+    <hyperlink ref="H22" r:id="rId61"/>
+    <hyperlink ref="M22" r:id="rId62" location="geoid=0700000US390493777299999"/>
+    <hyperlink ref="N22" r:id="rId63"/>
+    <hyperlink ref="H23" r:id="rId64"/>
+    <hyperlink ref="M23" r:id="rId65" location="geoid=0700000US390493861299999"/>
+    <hyperlink ref="N23" r:id="rId66"/>
+    <hyperlink ref="H24" r:id="rId67"/>
+    <hyperlink ref="M24" r:id="rId68" location="geoid=0700000US390494641099999"/>
+    <hyperlink ref="N24" r:id="rId69"/>
+    <hyperlink ref="H25" r:id="rId70"/>
+    <hyperlink ref="M25" r:id="rId71" location="geoid=0700000US390495006499999"/>
+    <hyperlink ref="N25" r:id="rId72"/>
+    <hyperlink ref="H26" r:id="rId73"/>
+    <hyperlink ref="M26" r:id="rId74" location="geoid=0700000US390496184099999"/>
+    <hyperlink ref="N26" r:id="rId75"/>
+    <hyperlink ref="H27" r:id="rId76"/>
+    <hyperlink ref="M27" r:id="rId77" location="geoid=0700000US390496297499999"/>
+    <hyperlink ref="N27" r:id="rId78"/>
+    <hyperlink ref="H28" r:id="rId79"/>
+    <hyperlink ref="M28" r:id="rId80" location="geoid=0700000US390496457099999"/>
+    <hyperlink ref="N28" r:id="rId81"/>
+    <hyperlink ref="H29" r:id="rId82"/>
+    <hyperlink ref="M29" r:id="rId83" location="geoid=0700000US390497771499999"/>
+    <hyperlink ref="N29" r:id="rId84"/>
+    <hyperlink ref="H30" r:id="rId85"/>
+    <hyperlink ref="M30" r:id="rId86" location="geoid=0700000US390498124299999"/>
+    <hyperlink ref="N30" r:id="rId87"/>
+    <hyperlink ref="H31" r:id="rId88"/>
+    <hyperlink ref="M31" r:id="rId89" location="geoid=0700000US390892569099999"/>
+    <hyperlink ref="N31" r:id="rId90"/>
+    <hyperlink ref="H32" r:id="rId91"/>
+    <hyperlink ref="M32" r:id="rId92" location="geoid=0700000US390893141699999"/>
+    <hyperlink ref="N32" r:id="rId93"/>
+    <hyperlink ref="H33" r:id="rId94"/>
+    <hyperlink ref="M33" r:id="rId95" location="geoid=0700000US391593904699999"/>
+    <hyperlink ref="N33" r:id="rId96"/>
+    <hyperlink ref="H34" r:id="rId97"/>
+    <hyperlink ref="M34" r:id="rId98" location="geoid=1600000US3905130"/>
+    <hyperlink ref="N34" r:id="rId99"/>
+    <hyperlink ref="H35" r:id="rId100"/>
+    <hyperlink ref="M35" r:id="rId101" location="geoid=1600000US3906278"/>
+    <hyperlink ref="N35" r:id="rId102"/>
+    <hyperlink ref="H36" r:id="rId103"/>
+    <hyperlink ref="M36" r:id="rId104" location="geoid=1600000US3909890"/>
+    <hyperlink ref="N36" r:id="rId105"/>
+    <hyperlink ref="H37" r:id="rId106"/>
+    <hyperlink ref="M37" r:id="rId107" location="geoid=1600000US3914184"/>
+    <hyperlink ref="N37" r:id="rId108"/>
+    <hyperlink ref="H38" r:id="rId109"/>
+    <hyperlink ref="M38" r:id="rId110" location="geoid=1600000US3915070"/>
+    <hyperlink ref="N38" r:id="rId111"/>
+    <hyperlink ref="H39" r:id="rId112"/>
+    <hyperlink ref="M39" r:id="rId113" location="geoid=1600000US3918000"/>
+    <hyperlink ref="N39" r:id="rId114"/>
+    <hyperlink ref="H40" r:id="rId115"/>
+    <hyperlink ref="M40" r:id="rId116" location="geoid=1600000US3921434"/>
+    <hyperlink ref="N40" r:id="rId117"/>
+    <hyperlink ref="H41" r:id="rId118"/>
+    <hyperlink ref="M41" r:id="rId119" location="geoid=1600000US3922694"/>
+    <hyperlink ref="N41" r:id="rId120"/>
+    <hyperlink ref="H42" r:id="rId121"/>
+    <hyperlink ref="M42" r:id="rId122" location="geoid=1600000US3929106"/>
+    <hyperlink ref="N42" r:id="rId123"/>
+    <hyperlink ref="H43" r:id="rId124"/>
+    <hyperlink ref="M43" r:id="rId125" location="geoid=1600000US3929148"/>
+    <hyperlink ref="N43" r:id="rId126"/>
+    <hyperlink ref="H44" r:id="rId127"/>
+    <hyperlink ref="M44" r:id="rId128" location="geoid=1600000US3929246"/>
+    <hyperlink ref="N44" r:id="rId129"/>
+    <hyperlink ref="H45" r:id="rId130"/>
+    <hyperlink ref="M45" r:id="rId131" location="geoid=1600000US3931304"/>
+    <hyperlink ref="N45" r:id="rId132"/>
+    <hyperlink ref="H46" r:id="rId133"/>
+    <hyperlink ref="M46" r:id="rId134" location="geoid=1600000US3931402"/>
+    <hyperlink ref="N46" r:id="rId135"/>
+    <hyperlink ref="H47" r:id="rId136"/>
+    <hyperlink ref="M47" r:id="rId137" location="geoid=1600000US3932592"/>
+    <hyperlink ref="N47" r:id="rId138"/>
+    <hyperlink ref="H48" r:id="rId139"/>
+    <hyperlink ref="M48" r:id="rId140" location="geoid=1600000US3932606"/>
+    <hyperlink ref="N48" r:id="rId141"/>
+    <hyperlink ref="H49" r:id="rId142"/>
+    <hyperlink ref="M49" r:id="rId143" location="geoid=1600000US3934748"/>
+    <hyperlink ref="N49" r:id="rId144"/>
+    <hyperlink ref="H50" r:id="rId145"/>
+    <hyperlink ref="M50" r:id="rId146" location="geoid=1600000US3934790"/>
+    <hyperlink ref="N50" r:id="rId147"/>
+    <hyperlink ref="H51" r:id="rId148"/>
+    <hyperlink ref="M51" r:id="rId149" location="geoid=1600000US3935476"/>
+    <hyperlink ref="N51" r:id="rId150"/>
+    <hyperlink ref="H52" r:id="rId151"/>
+    <hyperlink ref="M52" r:id="rId152" location="geoid=1600000US3939340"/>
+    <hyperlink ref="N52" r:id="rId153"/>
+    <hyperlink ref="H53" r:id="rId154"/>
+    <hyperlink ref="M53" r:id="rId155" location="geoid=1600000US3941720"/>
+    <hyperlink ref="N53" r:id="rId156"/>
+    <hyperlink ref="H54" r:id="rId157"/>
+    <hyperlink ref="M54" r:id="rId158" location="geoid=1600000US3944674"/>
+    <hyperlink ref="N54" r:id="rId159"/>
+    <hyperlink ref="H55" r:id="rId160"/>
+    <hyperlink ref="M55" r:id="rId161" location="geoid=1600000US3947474"/>
+    <hyperlink ref="N55" r:id="rId162"/>
+    <hyperlink ref="H56" r:id="rId163"/>
+    <hyperlink ref="M56" r:id="rId164" location="geoid=1600000US3947754"/>
+    <hyperlink ref="N56" r:id="rId165"/>
+    <hyperlink ref="H57" r:id="rId166"/>
+    <hyperlink ref="M57" r:id="rId167" location="geoid=1600000US3948160"/>
+    <hyperlink ref="N57" r:id="rId168"/>
+    <hyperlink ref="H58" r:id="rId169"/>
+    <hyperlink ref="M58" r:id="rId170" location="geoid=1600000US3950862"/>
+    <hyperlink ref="N58" r:id="rId171"/>
+    <hyperlink ref="H59" r:id="rId172"/>
+    <hyperlink ref="M59" r:id="rId173" location="geoid=1600000US3953046"/>
+    <hyperlink ref="N59" r:id="rId174"/>
+    <hyperlink ref="H60" r:id="rId175"/>
+    <hyperlink ref="M60" r:id="rId176" location="geoid=1600000US3953102"/>
+    <hyperlink ref="N60" r:id="rId177"/>
+    <hyperlink ref="H61" r:id="rId178"/>
+    <hyperlink ref="M61" r:id="rId179" location="geoid=1600000US3953970"/>
+    <hyperlink ref="N61" r:id="rId180"/>
+    <hyperlink ref="H62" r:id="rId181"/>
+    <hyperlink ref="M62" r:id="rId182" location="geoid=1600000US3954040"/>
+    <hyperlink ref="N62" r:id="rId183"/>
+    <hyperlink ref="H63" r:id="rId184"/>
+    <hyperlink ref="M63" r:id="rId185" location="geoid=1600000US3954866"/>
+    <hyperlink ref="N63" r:id="rId186"/>
+    <hyperlink ref="H64" r:id="rId187"/>
+    <hyperlink ref="M64" r:id="rId188" location="geoid=1600000US3957862"/>
+    <hyperlink ref="N64" r:id="rId189"/>
+    <hyperlink ref="H65" r:id="rId190"/>
+    <hyperlink ref="M65" r:id="rId191" location="geoid=1600000US3961112"/>
+    <hyperlink ref="N65" r:id="rId192"/>
+    <hyperlink ref="H66" r:id="rId193"/>
+    <hyperlink ref="M66" r:id="rId194" location="geoid=1600000US3962498"/>
+    <hyperlink ref="N66" r:id="rId195"/>
+    <hyperlink ref="H67" r:id="rId196"/>
+    <hyperlink ref="M67" r:id="rId197" location="geoid=1600000US3963030"/>
+    <hyperlink ref="N67" r:id="rId198"/>
+    <hyperlink ref="H68" r:id="rId199"/>
+    <hyperlink ref="M68" r:id="rId200" location="geoid=1600000US3964486"/>
+    <hyperlink ref="N68" r:id="rId201"/>
+    <hyperlink ref="H69" r:id="rId202"/>
+    <hyperlink ref="M69" r:id="rId203" location="geoid=1600000US3966390"/>
+    <hyperlink ref="N69" r:id="rId204"/>
+    <hyperlink ref="H70" r:id="rId205"/>
+    <hyperlink ref="M70" r:id="rId206" location="geoid=1600000US3967440"/>
+    <hyperlink ref="N70" r:id="rId207"/>
+    <hyperlink ref="H71" r:id="rId208"/>
+    <hyperlink ref="M71" r:id="rId209" location="geoid=1600000US3971976"/>
+    <hyperlink ref="N71" r:id="rId210"/>
+    <hyperlink ref="H72" r:id="rId211"/>
+    <hyperlink ref="M72" r:id="rId212" location="geoid=1600000US3972977"/>
+    <hyperlink ref="N72" r:id="rId213"/>
+    <hyperlink ref="H73" r:id="rId214"/>
+    <hyperlink ref="M73" r:id="rId215" location="geoid=1600000US3975602"/>
+    <hyperlink ref="N73" r:id="rId216"/>
+    <hyperlink ref="H74" r:id="rId217"/>
+    <hyperlink ref="M74" r:id="rId218" location="geoid=1600000US3979002"/>
+    <hyperlink ref="N74" r:id="rId219"/>
+    <hyperlink ref="H75" r:id="rId220"/>
+    <hyperlink ref="M75" r:id="rId221" location="geoid=1600000US3979100"/>
+    <hyperlink ref="N75" r:id="rId222"/>
+    <hyperlink ref="H76" r:id="rId223"/>
+    <hyperlink ref="M76" r:id="rId224" location="geoid=1600000US3983580"/>
+    <hyperlink ref="N76" r:id="rId225"/>
+    <hyperlink ref="H77" r:id="rId226"/>
+    <hyperlink ref="M77" r:id="rId227" location="geoid=1600000US3984742"/>
+    <hyperlink ref="N77" r:id="rId228"/>
+    <hyperlink ref="H78" r:id="rId229"/>
+    <hyperlink ref="M78" r:id="rId230" location="geoid=1600000US3986604"/>
+    <hyperlink ref="N78" r:id="rId231"/>
+    <hyperlink ref="H79" r:id="rId232"/>
+    <hyperlink ref="M79" r:id="rId233" location="geoid=M010000US001"/>
+    <hyperlink ref="N79" r:id="rId234"/>
+    <hyperlink ref="H80" r:id="rId235"/>
+    <hyperlink ref="M80" r:id="rId236" location="geoid=0500000US39041"/>
+    <hyperlink ref="N80" r:id="rId237"/>
+    <hyperlink ref="H81" r:id="rId238"/>
+    <hyperlink ref="M81" r:id="rId239" location="geoid=0500000US39045"/>
+    <hyperlink ref="N81" r:id="rId240"/>
+    <hyperlink ref="H82" r:id="rId241"/>
+    <hyperlink ref="M82" r:id="rId242" location="geoid=0500000US39047"/>
+    <hyperlink ref="N82" r:id="rId243"/>
+    <hyperlink ref="H83" r:id="rId244"/>
+    <hyperlink ref="M83" r:id="rId245" location="geoid=0500000US39049"/>
+    <hyperlink ref="N83" r:id="rId246"/>
+    <hyperlink ref="H84" r:id="rId247"/>
+    <hyperlink ref="M84" r:id="rId248" location="geoid=0500000US39073"/>
+    <hyperlink ref="N84" r:id="rId249"/>
+    <hyperlink ref="H85" r:id="rId250"/>
+    <hyperlink ref="M85" r:id="rId251" location="geoid=0500000US39083"/>
+    <hyperlink ref="N85" r:id="rId252"/>
+    <hyperlink ref="H86" r:id="rId253"/>
+    <hyperlink ref="M86" r:id="rId254" location="geoid=0500000US39089"/>
+    <hyperlink ref="N86" r:id="rId255"/>
+    <hyperlink ref="H87" r:id="rId256"/>
+    <hyperlink ref="M87" r:id="rId257" location="geoid=0500000US39091"/>
+    <hyperlink ref="N87" r:id="rId258"/>
+    <hyperlink ref="H88" r:id="rId259"/>
+    <hyperlink ref="M88" r:id="rId260" location="geoid=0500000US39097"/>
+    <hyperlink ref="N88" r:id="rId261"/>
+    <hyperlink ref="H89" r:id="rId262"/>
+    <hyperlink ref="M89" r:id="rId263" location="geoid=0500000US39101"/>
+    <hyperlink ref="N89" r:id="rId264"/>
+    <hyperlink ref="H90" r:id="rId265"/>
+    <hyperlink ref="M90" r:id="rId266" location="geoid=0500000US39117"/>
+    <hyperlink ref="N90" r:id="rId267"/>
+    <hyperlink ref="H91" r:id="rId268"/>
+    <hyperlink ref="M91" r:id="rId269" location="geoid=0500000US39127"/>
+    <hyperlink ref="N91" r:id="rId270"/>
+    <hyperlink ref="H92" r:id="rId271"/>
+    <hyperlink ref="M92" r:id="rId272" location="geoid=0500000US39129"/>
+    <hyperlink ref="N92" r:id="rId273"/>
+    <hyperlink ref="H93" r:id="rId274"/>
+    <hyperlink ref="M93" r:id="rId275" location="geoid=0500000US39141"/>
+    <hyperlink ref="N93" r:id="rId276"/>
+    <hyperlink ref="H94" r:id="rId277"/>
+    <hyperlink ref="M94" r:id="rId278" location="geoid=0500000US39159"/>
+    <hyperlink ref="N94" r:id="rId279"/>
+    <hyperlink ref="H95" r:id="rId280"/>
+    <hyperlink ref="M95" r:id="rId281" location="geoid=0700000US390458020699999"/>
+    <hyperlink ref="N95" r:id="rId282"/>
+    <hyperlink ref="H96" r:id="rId283"/>
+    <hyperlink ref="M96" r:id="rId284" location="geoid=0700000US390490692299999"/>
+    <hyperlink ref="N96" r:id="rId285"/>
+    <hyperlink ref="H97" r:id="rId286"/>
+    <hyperlink ref="M97" r:id="rId287" location="geoid=0700000US390490944299999"/>
+    <hyperlink ref="N97" r:id="rId288"/>
+    <hyperlink ref="H98" r:id="rId289"/>
+    <hyperlink ref="M98" r:id="rId290" location="geoid=0700000US390491611299999"/>
+    <hyperlink ref="N98" r:id="rId291"/>
+    <hyperlink ref="H99" r:id="rId292"/>
+    <hyperlink ref="M99" r:id="rId293" location="geoid=0700000US390492828099999"/>
+    <hyperlink ref="N99" r:id="rId294"/>
+    <hyperlink ref="H100" r:id="rId295"/>
+    <hyperlink ref="M100" r:id="rId296" location="geoid=0700000US390493777299999"/>
+    <hyperlink ref="N100" r:id="rId297"/>
+    <hyperlink ref="H101" r:id="rId298"/>
+    <hyperlink ref="M101" r:id="rId299" location="geoid=0700000US390493861299999"/>
+    <hyperlink ref="N101" r:id="rId300"/>
+    <hyperlink ref="H102" r:id="rId301"/>
+    <hyperlink ref="M102" r:id="rId302" location="geoid=0700000US390494641099999"/>
+    <hyperlink ref="N102" r:id="rId303"/>
+    <hyperlink ref="H103" r:id="rId304"/>
+    <hyperlink ref="M103" r:id="rId305" location="geoid=0700000US390495006499999"/>
+    <hyperlink ref="N103" r:id="rId306"/>
+    <hyperlink ref="H104" r:id="rId307"/>
+    <hyperlink ref="M104" r:id="rId308" location="geoid=0700000US390496184099999"/>
+    <hyperlink ref="N104" r:id="rId309"/>
+    <hyperlink ref="H105" r:id="rId310"/>
+    <hyperlink ref="M105" r:id="rId311" location="geoid=0700000US390496297499999"/>
+    <hyperlink ref="N105" r:id="rId312"/>
+    <hyperlink ref="H106" r:id="rId313"/>
+    <hyperlink ref="M106" r:id="rId314" location="geoid=0700000US390496457099999"/>
+    <hyperlink ref="N106" r:id="rId315"/>
+    <hyperlink ref="H107" r:id="rId316"/>
+    <hyperlink ref="M107" r:id="rId317" location="geoid=0700000US390497771499999"/>
+    <hyperlink ref="N107" r:id="rId318"/>
+    <hyperlink ref="H108" r:id="rId319"/>
+    <hyperlink ref="M108" r:id="rId320" location="geoid=0700000US390498124299999"/>
+    <hyperlink ref="N108" r:id="rId321"/>
+    <hyperlink ref="H109" r:id="rId322"/>
+    <hyperlink ref="M109" r:id="rId323" location="geoid=0700000US390892569099999"/>
+    <hyperlink ref="N109" r:id="rId324"/>
+    <hyperlink ref="H110" r:id="rId325"/>
+    <hyperlink ref="M110" r:id="rId326" location="geoid=0700000US390893141699999"/>
+    <hyperlink ref="N110" r:id="rId327"/>
+    <hyperlink ref="H111" r:id="rId328"/>
+    <hyperlink ref="M111" r:id="rId329" location="geoid=0700000US391593904699999"/>
+    <hyperlink ref="N111" r:id="rId330"/>
+    <hyperlink ref="H112" r:id="rId331"/>
+    <hyperlink ref="M112" r:id="rId332" location="geoid=1600000US3905130"/>
+    <hyperlink ref="N112" r:id="rId333"/>
+    <hyperlink ref="H113" r:id="rId334"/>
+    <hyperlink ref="M113" r:id="rId335" location="geoid=1600000US3906278"/>
+    <hyperlink ref="N113" r:id="rId336"/>
+    <hyperlink ref="H114" r:id="rId337"/>
+    <hyperlink ref="M114" r:id="rId338" location="geoid=1600000US3909890"/>
+    <hyperlink ref="N114" r:id="rId339"/>
+    <hyperlink ref="H115" r:id="rId340"/>
+    <hyperlink ref="M115" r:id="rId341" location="geoid=1600000US3914184"/>
+    <hyperlink ref="N115" r:id="rId342"/>
+    <hyperlink ref="H116" r:id="rId343"/>
+    <hyperlink ref="M116" r:id="rId344" location="geoid=1600000US3915070"/>
+    <hyperlink ref="N116" r:id="rId345"/>
+    <hyperlink ref="H117" r:id="rId346"/>
+    <hyperlink ref="M117" r:id="rId347" location="geoid=1600000US3918000"/>
+    <hyperlink ref="N117" r:id="rId348"/>
+    <hyperlink ref="H118" r:id="rId349"/>
+    <hyperlink ref="M118" r:id="rId350" location="geoid=1600000US3921434"/>
+    <hyperlink ref="N118" r:id="rId351"/>
+    <hyperlink ref="H119" r:id="rId352"/>
+    <hyperlink ref="M119" r:id="rId353" location="geoid=1600000US3922694"/>
+    <hyperlink ref="N119" r:id="rId354"/>
+    <hyperlink ref="H120" r:id="rId355"/>
+    <hyperlink ref="M120" r:id="rId356" location="geoid=1600000US3929106"/>
+    <hyperlink ref="N120" r:id="rId357"/>
+    <hyperlink ref="H121" r:id="rId358"/>
+    <hyperlink ref="M121" r:id="rId359" location="geoid=1600000US3929148"/>
+    <hyperlink ref="N121" r:id="rId360"/>
+    <hyperlink ref="H122" r:id="rId361"/>
+    <hyperlink ref="M122" r:id="rId362" location="geoid=1600000US3929246"/>
+    <hyperlink ref="N122" r:id="rId363"/>
+    <hyperlink ref="H123" r:id="rId364"/>
+    <hyperlink ref="M123" r:id="rId365" location="geoid=1600000US3931304"/>
+    <hyperlink ref="N123" r:id="rId366"/>
+    <hyperlink ref="H124" r:id="rId367"/>
+    <hyperlink ref="M124" r:id="rId368" location="geoid=1600000US3931402"/>
+    <hyperlink ref="N124" r:id="rId369"/>
+    <hyperlink ref="H125" r:id="rId370"/>
+    <hyperlink ref="M125" r:id="rId371" location="geoid=1600000US3932592"/>
+    <hyperlink ref="N125" r:id="rId372"/>
+    <hyperlink ref="H126" r:id="rId373"/>
+    <hyperlink ref="M126" r:id="rId374" location="geoid=1600000US3932606"/>
+    <hyperlink ref="N126" r:id="rId375"/>
+    <hyperlink ref="H127" r:id="rId376"/>
+    <hyperlink ref="M127" r:id="rId377" location="geoid=1600000US3934748"/>
+    <hyperlink ref="N127" r:id="rId378"/>
+    <hyperlink ref="H128" r:id="rId379"/>
+    <hyperlink ref="M128" r:id="rId380" location="geoid=1600000US3934790"/>
+    <hyperlink ref="N128" r:id="rId381"/>
+    <hyperlink ref="H129" r:id="rId382"/>
+    <hyperlink ref="M129" r:id="rId383" location="geoid=1600000US3935476"/>
+    <hyperlink ref="N129" r:id="rId384"/>
+    <hyperlink ref="H130" r:id="rId385"/>
+    <hyperlink ref="M130" r:id="rId386" location="geoid=1600000US3939340"/>
+    <hyperlink ref="N130" r:id="rId387"/>
+    <hyperlink ref="H131" r:id="rId388"/>
+    <hyperlink ref="M131" r:id="rId389" location="geoid=1600000US3941720"/>
+    <hyperlink ref="N131" r:id="rId390"/>
+    <hyperlink ref="H132" r:id="rId391"/>
+    <hyperlink ref="M132" r:id="rId392" location="geoid=1600000US3944674"/>
+    <hyperlink ref="N132" r:id="rId393"/>
+    <hyperlink ref="H133" r:id="rId394"/>
+    <hyperlink ref="M133" r:id="rId395" location="geoid=1600000US3947474"/>
+    <hyperlink ref="N133" r:id="rId396"/>
+    <hyperlink ref="H134" r:id="rId397"/>
+    <hyperlink ref="M134" r:id="rId398" location="geoid=1600000US3947754"/>
+    <hyperlink ref="N134" r:id="rId399"/>
+    <hyperlink ref="H135" r:id="rId400"/>
+    <hyperlink ref="M135" r:id="rId401" location="geoid=1600000US3948160"/>
+    <hyperlink ref="N135" r:id="rId402"/>
+    <hyperlink ref="H136" r:id="rId403"/>
+    <hyperlink ref="M136" r:id="rId404" location="geoid=1600000US3950862"/>
+    <hyperlink ref="N136" r:id="rId405"/>
+    <hyperlink ref="H137" r:id="rId406"/>
+    <hyperlink ref="M137" r:id="rId407" location="geoid=1600000US3953046"/>
+    <hyperlink ref="N137" r:id="rId408"/>
+    <hyperlink ref="H138" r:id="rId409"/>
+    <hyperlink ref="M138" r:id="rId410" location="geoid=1600000US3953102"/>
+    <hyperlink ref="N138" r:id="rId411"/>
+    <hyperlink ref="H139" r:id="rId412"/>
+    <hyperlink ref="M139" r:id="rId413" location="geoid=1600000US3953970"/>
+    <hyperlink ref="N139" r:id="rId414"/>
+    <hyperlink ref="H140" r:id="rId415"/>
+    <hyperlink ref="M140" r:id="rId416" location="geoid=1600000US3954040"/>
+    <hyperlink ref="N140" r:id="rId417"/>
+    <hyperlink ref="H141" r:id="rId418"/>
+    <hyperlink ref="M141" r:id="rId419" location="geoid=1600000US3954866"/>
+    <hyperlink ref="N141" r:id="rId420"/>
+    <hyperlink ref="H142" r:id="rId421"/>
+    <hyperlink ref="M142" r:id="rId422" location="geoid=1600000US3957862"/>
+    <hyperlink ref="N142" r:id="rId423"/>
+    <hyperlink ref="H143" r:id="rId424"/>
+    <hyperlink ref="M143" r:id="rId425" location="geoid=1600000US3961112"/>
+    <hyperlink ref="N143" r:id="rId426"/>
+    <hyperlink ref="H144" r:id="rId427"/>
+    <hyperlink ref="M144" r:id="rId428" location="geoid=1600000US3962498"/>
+    <hyperlink ref="N144" r:id="rId429"/>
+    <hyperlink ref="H145" r:id="rId430"/>
+    <hyperlink ref="M145" r:id="rId431" location="geoid=1600000US3963030"/>
+    <hyperlink ref="N145" r:id="rId432"/>
+    <hyperlink ref="H146" r:id="rId433"/>
+    <hyperlink ref="M146" r:id="rId434" location="geoid=1600000US3964486"/>
+    <hyperlink ref="N146" r:id="rId435"/>
+    <hyperlink ref="H147" r:id="rId436"/>
+    <hyperlink ref="M147" r:id="rId437" location="geoid=1600000US3966390"/>
+    <hyperlink ref="N147" r:id="rId438"/>
+    <hyperlink ref="H148" r:id="rId439"/>
+    <hyperlink ref="M148" r:id="rId440" location="geoid=1600000US3967440"/>
+    <hyperlink ref="N148" r:id="rId441"/>
+    <hyperlink ref="H149" r:id="rId442"/>
+    <hyperlink ref="M149" r:id="rId443" location="geoid=1600000US3971976"/>
+    <hyperlink ref="N149" r:id="rId444"/>
+    <hyperlink ref="H150" r:id="rId445"/>
+    <hyperlink ref="M150" r:id="rId446" location="geoid=1600000US3972977"/>
+    <hyperlink ref="N150" r:id="rId447"/>
+    <hyperlink ref="H151" r:id="rId448"/>
+    <hyperlink ref="M151" r:id="rId449" location="geoid=1600000US3975602"/>
+    <hyperlink ref="N151" r:id="rId450"/>
+    <hyperlink ref="H152" r:id="rId451"/>
+    <hyperlink ref="M152" r:id="rId452" location="geoid=1600000US3979002"/>
+    <hyperlink ref="N152" r:id="rId453"/>
+    <hyperlink ref="H153" r:id="rId454"/>
+    <hyperlink ref="M153" r:id="rId455" location="geoid=1600000US3979100"/>
+    <hyperlink ref="N153" r:id="rId456"/>
+    <hyperlink ref="H154" r:id="rId457"/>
+    <hyperlink ref="M154" r:id="rId458" location="geoid=1600000US3983580"/>
+    <hyperlink ref="N154" r:id="rId459"/>
+    <hyperlink ref="H155" r:id="rId460"/>
+    <hyperlink ref="M155" r:id="rId461" location="geoid=1600000US3984742"/>
+    <hyperlink ref="N155" r:id="rId462"/>
+    <hyperlink ref="H156" r:id="rId463"/>
+    <hyperlink ref="M156" r:id="rId464" location="geoid=1600000US3986604"/>
+    <hyperlink ref="N156" r:id="rId465"/>
+    <hyperlink ref="H157" r:id="rId466"/>
+    <hyperlink ref="M157" r:id="rId467" location="geoid=M010000US001"/>
+    <hyperlink ref="N157" r:id="rId468"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>